<commit_message>
V4 finished, add Redis
</commit_message>
<xml_diff>
--- a/src/main/resources/网站数据.xlsx
+++ b/src/main/resources/网站数据.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\javalearning\Projectmobi\mobi-backend\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C00BFB-9F3B-4169-B3C7-625AA9BF5E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3E25B8-0EA1-44E4-A0FE-F74D6680BCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11300" yWindow="1400" windowWidth="12640" windowHeight="11870" xr2:uid="{229EEA6E-F8A7-2545-904A-8F0032855BE1}"/>
+    <workbookView xWindow="3830" yWindow="1530" windowWidth="12640" windowHeight="11870" xr2:uid="{229EEA6E-F8A7-2545-904A-8F0032855BE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>日期</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -73,6 +73,141 @@
         <sz val="10"/>
         <rFont val="宋体"/>
         <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>号</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>号</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>号</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>号</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>号</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>号</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>号</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>号</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>号</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="等线"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>号</t>
@@ -87,7 +222,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy/m/d\ h:mm;@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="18"/>
       <color theme="1"/>
@@ -129,6 +264,12 @@
     <font>
       <sz val="10"/>
       <name val="Microsoft YaHei UI"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
     </font>
@@ -481,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{260829AF-83D5-9D43-A57C-13A2BDCFFDE0}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="22.5"/>
@@ -528,6 +669,78 @@
         <v>50</v>
       </c>
     </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>